<commit_message>
Added custom generator and tests
</commit_message>
<xml_diff>
--- a/tests/Libro3.xlsx
+++ b/tests/Libro3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="66">
   <si>
     <t>Test1</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>/home/user/datasets/dataset_solar/poly/Luka_version_train_only_big_defective/train</t>
-  </si>
-  <si>
     <t>final_activation</t>
   </si>
   <si>
@@ -152,21 +149,95 @@
     <t>Test16_base_comparison_2</t>
   </si>
   <si>
-    <t>/home/user/datasets/dataset_solar/poly/Luka_version_train_only_defective/train</t>
-  </si>
-  <si>
     <t>Test16_base_comparison_3</t>
   </si>
   <si>
-    <t>noAHE</t>
+    <t>Test17</t>
+  </si>
+  <si>
+    <t>aug</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>/home/jbalzategi/datasets/dataset_solar/poly/Luka_version_train_only_big_defective/train</t>
+  </si>
+  <si>
+    <t>/home/jbalzategi/datasets/dataset_solar/poly/Luka_version_train_only_defective/train</t>
+  </si>
+  <si>
+    <t>unet_deconv</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>Test18</t>
+  </si>
+  <si>
+    <t>Test19</t>
+  </si>
+  <si>
+    <t>/home/jbalzategi/datasets/dataset_solar/poly/Luka_version_train_only_defective_manual_augmented/train</t>
+  </si>
+  <si>
+    <t>Test20</t>
+  </si>
+  <si>
+    <t>unet /deconv</t>
+  </si>
+  <si>
+    <t>rotation/None</t>
+  </si>
+  <si>
+    <t>defective/ aug</t>
+  </si>
+  <si>
+    <t>unet + aug 17</t>
+  </si>
+  <si>
+    <t>unet + rota 18</t>
+  </si>
+  <si>
+    <t>deconv 19</t>
+  </si>
+  <si>
+    <t>deconv + rota 20</t>
+  </si>
+  <si>
+    <t>Test21</t>
+  </si>
+  <si>
+    <t>deconv + aug 21</t>
+  </si>
+  <si>
+    <t>Titan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPU </t>
+  </si>
+  <si>
+    <t>Geforce</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -194,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -211,6 +282,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,13 +575,10 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="12" width="10.77734375" customWidth="1"/>
     <col min="13" max="13" width="24.6640625" customWidth="1"/>
-    <col min="14" max="14" width="72.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.44140625" customWidth="1"/>
-    <col min="16" max="16" width="49.77734375" customWidth="1"/>
-    <col min="17" max="17" width="37.88671875" customWidth="1"/>
+    <col min="14" max="20" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -543,65 +613,93 @@
         <v>33</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="R2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -639,17 +737,31 @@
         <v>33</v>
       </c>
       <c r="M3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -695,9 +807,23 @@
       <c r="O4" s="1">
         <v>1E-4</v>
       </c>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -743,9 +869,23 @@
       <c r="O5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -791,9 +931,23 @@
       <c r="O6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -839,10 +993,23 @@
       <c r="O7" s="2">
         <v>400</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P7" s="2">
+        <v>400</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>400</v>
+      </c>
+      <c r="R7" s="2">
+        <v>400</v>
+      </c>
+      <c r="S7" s="2">
+        <v>400</v>
+      </c>
+      <c r="T7" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -888,9 +1055,23 @@
       <c r="O8" s="2">
         <v>600</v>
       </c>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P8" s="2">
+        <v>600</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>600</v>
+      </c>
+      <c r="R8" s="2">
+        <v>600</v>
+      </c>
+      <c r="S8" s="2">
+        <v>600</v>
+      </c>
+      <c r="T8" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -936,9 +1117,23 @@
       <c r="O9" s="3">
         <v>50</v>
       </c>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P9" s="3">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>50</v>
+      </c>
+      <c r="R9" s="3">
+        <v>50</v>
+      </c>
+      <c r="S9" s="3">
+        <v>50</v>
+      </c>
+      <c r="T9" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -984,9 +1179,23 @@
       <c r="O10" s="2">
         <v>4</v>
       </c>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P10" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>4</v>
+      </c>
+      <c r="R10" s="2">
+        <v>4</v>
+      </c>
+      <c r="S10" s="2">
+        <v>4</v>
+      </c>
+      <c r="T10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1032,9 +1241,23 @@
       <c r="O11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1080,9 +1303,23 @@
       <c r="O12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1128,9 +1365,23 @@
       <c r="O13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1176,105 +1427,147 @@
       <c r="O14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1311,18 +1604,32 @@
       <c r="L17" s="2">
         <v>60</v>
       </c>
-      <c r="M17" s="2">
-        <v>62</v>
-      </c>
-      <c r="N17" s="2">
+      <c r="M17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q17" s="2">
         <v>107</v>
       </c>
-      <c r="O17" s="2">
-        <v>107</v>
-      </c>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S17" s="2">
+        <v>108</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1360,20 +1667,223 @@
         <v>23</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="O19" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" t="s">
+        <v>62</v>
+      </c>
+      <c r="L22" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" t="s">
+        <v>62</v>
+      </c>
+      <c r="O22" t="s">
+        <v>62</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="S22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P24" s="6"/>
+      <c r="R24" t="s">
+        <v>53</v>
+      </c>
+      <c r="S24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P25" s="6"/>
+      <c r="R25" t="s">
+        <v>54</v>
+      </c>
+      <c r="S25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P26" s="6"/>
+      <c r="R26" t="s">
+        <v>55</v>
+      </c>
+      <c r="S26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P27" s="6"/>
+      <c r="S27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P28" s="6"/>
+      <c r="S28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P29" s="6"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P30" s="6"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P31" s="6"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P36" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed little error on augmentation function: was only necessary to apply expand_dims on mask if rotation augmenation was applied
</commit_message>
<xml_diff>
--- a/tests/Libro3.xlsx
+++ b/tests/Libro3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="65">
   <si>
     <t>Test1</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>Geforce</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -566,8 +563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +682,7 @@
         <v>38</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>34</v>
@@ -1076,61 +1074,80 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <v>50</v>
+        <f t="shared" ref="B9:F9" si="0">B17/B10</f>
+        <v>1</v>
       </c>
       <c r="C9" s="3">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E9" s="3">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="F9" s="3">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="G9" s="3">
-        <v>50</v>
+        <f>G17/G10</f>
+        <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>50</v>
+        <f t="shared" ref="H9:T9" si="1">H17/H10</f>
+        <v>10</v>
       </c>
       <c r="I9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="J9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="K9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="L9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="M9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>53.5</v>
       </c>
       <c r="N9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>53.5</v>
       </c>
       <c r="O9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>26.75</v>
       </c>
       <c r="P9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>26.75</v>
       </c>
       <c r="Q9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>26.75</v>
       </c>
       <c r="R9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>26.75</v>
       </c>
       <c r="S9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>26.75</v>
       </c>
       <c r="T9" s="3">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>26.75</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1604,29 +1621,29 @@
       <c r="L17" s="2">
         <v>60</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>65</v>
+      <c r="M17" s="2">
+        <v>107</v>
+      </c>
+      <c r="N17" s="2">
+        <v>107</v>
+      </c>
+      <c r="O17" s="2">
+        <v>107</v>
+      </c>
+      <c r="P17" s="2">
+        <v>107</v>
       </c>
       <c r="Q17" s="2">
         <v>107</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>65</v>
+      <c r="R17" s="2">
+        <v>107</v>
       </c>
       <c r="S17" s="2">
-        <v>108</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>65</v>
+        <v>107</v>
+      </c>
+      <c r="T17" s="2">
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -1679,7 +1696,7 @@
         <v>37</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="R18" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Normalized dice loss to batch, read mask/gt as grayscale image
</commit_message>
<xml_diff>
--- a/tests/Libro3.xlsx
+++ b/tests/Libro3.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="sii2020" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="70">
   <si>
     <t>Test1</t>
   </si>
@@ -219,22 +220,29 @@
   </si>
   <si>
     <t>Geforce</t>
+  </si>
+  <si>
+    <t>unet_reduced</t>
+  </si>
+  <si>
+    <t>unet_pretrained</t>
+  </si>
+  <si>
+    <t>/home/jbalzategi/experiments/vgg16_weights_tf_dim_ordering_tf_kernels_notop.h5</t>
+  </si>
+  <si>
+    <t>Unet_orig</t>
+  </si>
+  <si>
+    <t>Unet_orig had bad results --&gt; the new_orig in the folder in dropbox is the test16_base_comparison_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -262,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -280,7 +288,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,11 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P3" sqref="P3"/>
+      <selection pane="topRight" activeCell="U32" sqref="U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,13 +692,13 @@
         <v>38</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>34</v>
@@ -1054,19 +1061,19 @@
         <v>600</v>
       </c>
       <c r="P8" s="2">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="Q8" s="2">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="R8" s="2">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="S8" s="2">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="T8" s="2">
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1074,80 +1081,66 @@
         <v>14</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" ref="B9:F9" si="0">B17/B10</f>
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3">
-        <f>G17/G10</f>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" ref="H9:T9" si="1">H17/H10</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="1"/>
-        <v>53.5</v>
+        <v>50</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" si="1"/>
-        <v>53.5</v>
+        <v>50</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="P9" s="3">
+        <f>P17/P10</f>
+        <v>56.75</v>
+      </c>
+      <c r="Q9" s="3">
+        <f>Q17/Q10</f>
         <v>26.75</v>
       </c>
-      <c r="P9" s="3">
-        <f t="shared" si="1"/>
+      <c r="R9" s="3">
+        <f>R17/R10</f>
         <v>26.75</v>
       </c>
-      <c r="Q9" s="3">
-        <f t="shared" si="1"/>
+      <c r="S9" s="3">
+        <f>S17/S10</f>
         <v>26.75</v>
       </c>
-      <c r="R9" s="3">
-        <f t="shared" si="1"/>
-        <v>26.75</v>
-      </c>
-      <c r="S9" s="3">
-        <f t="shared" si="1"/>
-        <v>26.75</v>
-      </c>
       <c r="T9" s="3">
-        <f t="shared" si="1"/>
-        <v>26.75</v>
+        <f>T17/T10</f>
+        <v>56.75</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1584,7 +1577,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1631,7 +1624,7 @@
         <v>107</v>
       </c>
       <c r="P17" s="2">
-        <v>107</v>
+        <v>227</v>
       </c>
       <c r="Q17" s="2">
         <v>107</v>
@@ -1643,10 +1636,10 @@
         <v>107</v>
       </c>
       <c r="T17" s="2">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1708,7 +1701,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1770,10 +1763,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1834,12 +1827,11 @@
       <c r="T22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="U22" s="7"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P24" s="6"/>
       <c r="R24" t="s">
         <v>53</v>
@@ -1848,7 +1840,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P25" s="6"/>
       <c r="R25" t="s">
         <v>54</v>
@@ -1857,7 +1849,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P26" s="6"/>
       <c r="R26" t="s">
         <v>55</v>
@@ -1866,28 +1858,32 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P27" s="6"/>
       <c r="S27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P28" s="6"/>
       <c r="S28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T28" t="e">
+        <f>+N23UA23:T28</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="P32" s="6"/>
     </row>
     <row r="33" spans="16:16" x14ac:dyDescent="0.3">
@@ -1906,4 +1902,412 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="73.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>400</v>
+      </c>
+      <c r="C7" s="2">
+        <v>400</v>
+      </c>
+      <c r="D7" s="2">
+        <v>400</v>
+      </c>
+      <c r="E7" s="2">
+        <v>400</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>500</v>
+      </c>
+      <c r="C8" s="2">
+        <v>500</v>
+      </c>
+      <c r="D8" s="2">
+        <v>500</v>
+      </c>
+      <c r="E8" s="2">
+        <v>600</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <v>50</v>
+      </c>
+      <c r="E9" s="3">
+        <v>50</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>107</v>
+      </c>
+      <c r="C17" s="2">
+        <v>107</v>
+      </c>
+      <c r="D17" s="2">
+        <v>107</v>
+      </c>
+      <c r="E17" s="2">
+        <v>107</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>